<commit_message>
recreated the test scripts
</commit_message>
<xml_diff>
--- a/2024 S1 Celseq2 Samlpe Generator/data/plate_spreadsheet_template.xlsx
+++ b/2024 S1 Celseq2 Samlpe Generator/data/plate_spreadsheet_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Genomics-Metadata-Multiplexing\test\input_files\op1.plate_layout_to_spreadsheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Genomics-Metadata-Multiplexing\2024 S1 Celseq2 Samlpe Generator\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BDDB54-C8F6-4943-BAB2-FDCA8BEC0C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEFDE56-42D5-439E-93A4-52E3408268D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33705" yWindow="750" windowWidth="32040" windowHeight="20130" xr2:uid="{E5692559-4AE4-9B44-98DF-B853A533C26D}"/>
+    <workbookView xWindow="2490" yWindow="300" windowWidth="32040" windowHeight="20130" xr2:uid="{E5692559-4AE4-9B44-98DF-B853A533C26D}"/>
   </bookViews>
   <sheets>
     <sheet name="LCE123" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t xml:space="preserve">Collaboration : </t>
   </si>
@@ -127,6 +127,10 @@
   </si>
   <si>
     <t>NKC_085</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ref_Ctrl</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
@@ -752,7 +756,7 @@
   <dimension ref="A1:AD74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -1522,7 +1526,7 @@
     <row r="33" spans="1:26" ht="21.95" customHeight="1">
       <c r="A33" s="27"/>
       <c r="B33" s="26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="X33" s="28"/>
     </row>
@@ -1535,7 +1539,7 @@
     <row r="35" spans="1:26" s="21" customFormat="1" ht="21.95" customHeight="1">
       <c r="A35" s="30"/>
       <c r="B35" s="26" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C35" s="31"/>
       <c r="D35" s="31"/>

</xml_diff>